<commit_message>
Update (Removed Auto Arima)
</commit_message>
<xml_diff>
--- a/Sufficient data/forecast_summary_B083NK82QJ.xlsx
+++ b/Sufficient data/forecast_summary_B083NK82QJ.xlsx
@@ -484,16 +484,16 @@
         <v>17</v>
       </c>
       <c r="D2" t="n">
-        <v/>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -519,16 +519,16 @@
         <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v/>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -554,16 +554,16 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v/>
+        <v>9</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G4" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -589,16 +589,16 @@
         <v>27</v>
       </c>
       <c r="D5" t="n">
-        <v/>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G5" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -624,16 +624,16 @@
         <v>24</v>
       </c>
       <c r="D6" t="n">
-        <v/>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G6" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -659,16 +659,16 @@
         <v>21</v>
       </c>
       <c r="D7" t="n">
-        <v/>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F7" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -694,16 +694,16 @@
         <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v/>
+        <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -729,16 +729,16 @@
         <v>29</v>
       </c>
       <c r="D9" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G9" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -764,16 +764,16 @@
         <v>33</v>
       </c>
       <c r="D10" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G10" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -799,16 +799,16 @@
         <v>29</v>
       </c>
       <c r="D11" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G11" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -834,16 +834,16 @@
         <v>18</v>
       </c>
       <c r="D12" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G12" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -869,16 +869,16 @@
         <v>9</v>
       </c>
       <c r="D13" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G13" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -904,16 +904,16 @@
         <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G14" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -939,16 +939,16 @@
         <v>13</v>
       </c>
       <c r="D15" t="n">
-        <v/>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G15" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -974,16 +974,16 @@
         <v>21</v>
       </c>
       <c r="D16" t="n">
-        <v/>
+        <v>8</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G16" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1009,16 +1009,16 @@
         <v>23</v>
       </c>
       <c r="D17" t="n">
-        <v/>
+        <v>7</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G17" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>

</xml_diff>